<commit_message>
fix cleaning, import test_a correct, change how data are mapped (removed apply_func)
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="151"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28260" tabRatio="151"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="91">
   <si>
     <t>521 Elm Street</t>
   </si>
@@ -250,6 +250,48 @@
   </si>
   <si>
     <t>pm_parent_property_id</t>
+  </si>
+  <si>
+    <t>extra_data_1</t>
+  </si>
+  <si>
+    <t>extra_data_2</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
   </si>
 </sst>
 </file>
@@ -329,9 +371,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="26">
+  <cellStyleXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -393,7 +437,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="26">
+  <cellStyles count="28">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -407,6 +451,7 @@
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -419,6 +464,7 @@
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -755,7 +801,7 @@
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -775,7 +821,7 @@
     <col min="17" max="17" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="11" customFormat="1" ht="12">
+    <row r="1" spans="1:20" s="11" customFormat="1" ht="24">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
@@ -827,8 +873,12 @@
       <c r="Q1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
+      <c r="R1" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>78</v>
+      </c>
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" s="1" customFormat="1">
@@ -878,8 +928,12 @@
       <c r="Q2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
+      <c r="R2" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="S2" s="4">
+        <v>1</v>
+      </c>
       <c r="T2" s="4"/>
     </row>
     <row r="3" spans="1:20" s="1" customFormat="1">
@@ -928,8 +982,12 @@
       <c r="Q3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
+      <c r="R3" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="S3" s="4">
+        <v>2</v>
+      </c>
       <c r="T3" s="4"/>
     </row>
     <row r="4" spans="1:20" s="1" customFormat="1">
@@ -978,8 +1036,12 @@
       <c r="Q4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
+      <c r="R4" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="S4" s="4">
+        <v>3</v>
+      </c>
       <c r="T4" s="4"/>
     </row>
     <row r="5" spans="1:20" s="1" customFormat="1">
@@ -1029,8 +1091,12 @@
       <c r="Q5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
+      <c r="R5" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="S5" s="4">
+        <v>4</v>
+      </c>
       <c r="T5" s="4"/>
     </row>
     <row r="6" spans="1:20" s="1" customFormat="1">
@@ -1080,8 +1146,12 @@
       <c r="Q6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
+      <c r="R6" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="S6" s="4">
+        <v>5</v>
+      </c>
       <c r="T6" s="4"/>
     </row>
     <row r="7" spans="1:20">
@@ -1134,8 +1204,12 @@
       <c r="Q7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
+      <c r="R7" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="S7" s="4">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="1">
@@ -1187,8 +1261,12 @@
       <c r="Q8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
+      <c r="R8" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="S8" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="1">
@@ -1240,8 +1318,12 @@
       <c r="Q9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
+      <c r="R9" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="S9" s="4">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" spans="1:20" ht="28">
       <c r="A10" s="1">
@@ -1293,8 +1375,12 @@
       <c r="Q10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
+      <c r="R10" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="S10" s="4">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" s="1">
@@ -1346,8 +1432,12 @@
       <c r="Q11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
+      <c r="R11" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="S11" s="4">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="1">
@@ -1399,8 +1489,12 @@
       <c r="Q12" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
+      <c r="R12" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="S12" s="4">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="1">
@@ -1447,6 +1541,12 @@
       </c>
       <c r="Q13" s="4" t="s">
         <v>74</v>
+      </c>
+      <c r="R13" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="S13" s="4">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add data_state, import_file to taxlot
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28260" tabRatio="151"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="151"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>building_portfolio_manager_identifier</t>
-  </si>
-  <si>
     <t>address_line_1</t>
   </si>
   <si>
@@ -246,9 +243,6 @@
     <t>Property record without Tax Record</t>
   </si>
   <si>
-    <t>jurisdiction_taxlot_identifier</t>
-  </si>
-  <si>
     <t>pm_parent_property_id</t>
   </si>
   <si>
@@ -292,6 +286,12 @@
   </si>
   <si>
     <t>l</t>
+  </si>
+  <si>
+    <t>pm_property_id</t>
+  </si>
+  <si>
+    <t>jurisdiction_tax_lot_id</t>
   </si>
 </sst>
 </file>
@@ -801,7 +801,7 @@
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -826,28 +826,28 @@
         <v>9</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="G1" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>4</v>
@@ -862,22 +862,22 @@
         <v>8</v>
       </c>
       <c r="N1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="R1" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="S1" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="T1" s="15"/>
     </row>
@@ -890,19 +890,19 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H2" s="3">
         <v>1552813</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J2" s="3">
         <v>75</v>
@@ -917,19 +917,19 @@
         <v>12555</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="S2" s="4">
         <v>1</v>
@@ -944,19 +944,19 @@
         <v>3020139</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H3" s="3">
         <v>11160509</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J3" s="3">
         <v>1</v>
@@ -971,19 +971,19 @@
         <v>513852</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="S3" s="4">
         <v>2</v>
@@ -998,25 +998,25 @@
         <v>4828379</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H4" s="3">
         <v>11160509</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L4" s="5">
         <v>42369</v>
@@ -1025,19 +1025,19 @@
         <v>55121</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="S4" s="4">
         <v>3</v>
@@ -1053,19 +1053,19 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="G5" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H5" s="3">
         <v>11160509</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J5" s="3">
         <v>63</v>
@@ -1080,19 +1080,19 @@
         <v>23543</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="S5" s="4">
         <v>4</v>
@@ -1108,19 +1108,19 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J6" s="3">
         <v>55</v>
@@ -1135,19 +1135,19 @@
         <v>200000</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="S6" s="4">
         <v>5</v>
@@ -1166,46 +1166,46 @@
         <v>1311523</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H7" s="4">
         <v>24651456</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L7" s="5">
         <v>42369</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P7" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="S7" s="4">
         <v>6</v>
@@ -1223,19 +1223,19 @@
         <v>1311523</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H8" s="4">
         <v>24651456</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J8" s="3">
         <v>77</v>
@@ -1250,19 +1250,19 @@
         <v>124523</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P8" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="S8" s="4">
         <v>7</v>
@@ -1280,19 +1280,19 @@
         <v>1311523</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H9" s="4">
         <v>24651456</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J9" s="3">
         <v>43</v>
@@ -1307,19 +1307,19 @@
         <v>421351</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P9" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R9" s="9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="S9" s="4">
         <v>8</v>
@@ -1337,19 +1337,19 @@
         <v>1311523</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H10" s="4">
         <v>24651456</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J10" s="3">
         <v>59</v>
@@ -1364,19 +1364,19 @@
         <v>1234</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P10" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R10" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="S10" s="4">
         <v>9</v>
@@ -1394,19 +1394,19 @@
         <v>1311523</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="J11" s="3">
         <v>34</v>
@@ -1421,19 +1421,19 @@
         <v>45324</v>
       </c>
       <c r="N11" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P11" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R11" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="S11" s="4">
         <v>10</v>
@@ -1451,25 +1451,25 @@
         <v>1311523</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="G12" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="K12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L12" s="5">
         <v>42369</v>
@@ -1478,19 +1478,19 @@
         <v>482215</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P12" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R12" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S12" s="4">
         <v>11</v>
@@ -1504,19 +1504,19 @@
         <v>6798215</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="J13" s="3">
         <v>88</v>
@@ -1531,19 +1531,19 @@
         <v>24523</v>
       </c>
       <c r="N13" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="O13" t="s">
         <v>71</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="P13" s="8" t="s">
+      <c r="Q13" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="Q13" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="R13" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="S13" s="4">
         <v>12</v>

</xml_diff>

<commit_message>
break out tests for handle_id_matches and query_property_matches
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="151"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="92">
   <si>
     <t>521 Elm Street</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>jurisdiction_tax_lot_id</t>
+  </si>
+  <si>
+    <t>custom_id_1</t>
   </si>
 </sst>
 </file>
@@ -371,9 +374,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="28">
+  <cellStyleXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -437,7 +448,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="28">
+  <cellStyles count="36">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -452,6 +463,10 @@
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -465,6 +480,10 @@
     <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -798,768 +817,807 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T13"/>
+  <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" customWidth="1"/>
-    <col min="8" max="8" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" customWidth="1"/>
-    <col min="10" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.1640625" customWidth="1"/>
-    <col min="13" max="13" width="11.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="13.5" style="8" customWidth="1"/>
-    <col min="17" max="17" width="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.83203125" customWidth="1"/>
+    <col min="9" max="9" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.83203125" customWidth="1"/>
+    <col min="11" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.1640625" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="13.5" style="8" customWidth="1"/>
+    <col min="18" max="18" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="11" customFormat="1" ht="24">
+    <row r="1" spans="1:21" s="11" customFormat="1" ht="24">
       <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
     </row>
-    <row r="2" spans="1:20" s="1" customFormat="1">
+    <row r="2" spans="1:21" s="1" customFormat="1">
       <c r="A2" s="1">
         <v>22</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
         <v>2264</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <v>1552813</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="3">
+      <c r="K2" s="3">
         <v>75</v>
       </c>
-      <c r="K2" s="3">
+      <c r="L2" s="3">
         <v>125</v>
       </c>
-      <c r="L2" s="5">
+      <c r="M2" s="5">
         <v>42369</v>
       </c>
-      <c r="M2" s="9">
+      <c r="N2" s="9">
         <v>12555</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="S2" s="4">
+      <c r="T2" s="4">
         <v>1</v>
       </c>
-      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
     </row>
-    <row r="3" spans="1:20" s="1" customFormat="1">
+    <row r="3" spans="1:21" s="1" customFormat="1">
       <c r="A3" s="1">
         <v>31</v>
       </c>
       <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
         <v>3020139</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <v>11160509</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="3">
+      <c r="K3" s="3">
         <v>1</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L3" s="3">
         <v>652.29999999999995</v>
       </c>
-      <c r="L3" s="5">
+      <c r="M3" s="5">
         <v>42369</v>
       </c>
-      <c r="M3" s="9">
+      <c r="N3" s="9">
         <v>513852</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="O3" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="Q3" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="R3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="S3" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="S3" s="4">
+      <c r="T3" s="4">
         <v>2</v>
       </c>
-      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
     </row>
-    <row r="4" spans="1:20" s="1" customFormat="1">
+    <row r="4" spans="1:21" s="1" customFormat="1">
       <c r="A4" s="1">
         <v>32</v>
       </c>
       <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
         <v>4828379</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>11160509</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="5">
         <v>42369</v>
       </c>
-      <c r="M4" s="9">
+      <c r="N4" s="9">
         <v>55121</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="O4" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="Q4" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="R4" s="9" t="s">
+      <c r="S4" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="S4" s="4">
+      <c r="T4" s="4">
         <v>3</v>
       </c>
-      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
     </row>
-    <row r="5" spans="1:20" s="1" customFormat="1">
+    <row r="5" spans="1:21" s="1" customFormat="1">
       <c r="A5" s="1">
         <v>33</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2">
         <v>1154623</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>11160509</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="3">
+      <c r="K5" s="3">
         <v>63</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
         <v>1202</v>
       </c>
-      <c r="L5" s="5">
+      <c r="M5" s="5">
         <v>42369</v>
       </c>
-      <c r="M5" s="9">
+      <c r="N5" s="9">
         <v>23543</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="O5" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="Q5" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="R5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="S5" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="S5" s="4">
+      <c r="T5" s="4">
         <v>4</v>
       </c>
-      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
     </row>
-    <row r="6" spans="1:20" s="1" customFormat="1">
+    <row r="6" spans="1:21" s="1" customFormat="1">
       <c r="A6" s="1">
         <v>50</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
         <v>5233255</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="3">
+      <c r="K6" s="3">
         <v>55</v>
       </c>
-      <c r="K6" s="3">
+      <c r="L6" s="3">
         <v>1358</v>
       </c>
-      <c r="L6" s="5">
+      <c r="M6" s="5">
         <v>42369</v>
       </c>
-      <c r="M6" s="9">
+      <c r="N6" s="9">
         <v>200000</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="O6" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="P6" s="9" t="s">
+      <c r="Q6" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="Q6" s="4" t="s">
+      <c r="R6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="S6" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="S6" s="4">
+      <c r="T6" s="4">
         <v>5</v>
       </c>
-      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:21">
       <c r="A7" s="1">
         <v>60</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="10">
+      <c r="C7" s="1">
+        <v>6</v>
+      </c>
+      <c r="D7" s="10">
         <v>1311523</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>1311523</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="4">
+      <c r="I7" s="4">
         <v>24651456</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M7" s="5">
         <v>42369</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="O7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P7" s="12" t="s">
+      <c r="Q7" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="Q7" s="4" t="s">
+      <c r="R7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="R7" s="9" t="s">
+      <c r="S7" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="S7" s="4">
+      <c r="T7" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:21">
       <c r="A8" s="1">
         <v>61</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2">
         <v>1311524</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>1311523</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="4">
+      <c r="I8" s="4">
         <v>24651456</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="3">
+      <c r="K8" s="3">
         <v>77</v>
       </c>
-      <c r="K8" s="3">
+      <c r="L8" s="3">
         <v>219</v>
       </c>
-      <c r="L8" s="5">
+      <c r="M8" s="5">
         <v>42369</v>
       </c>
-      <c r="M8" s="13">
+      <c r="N8" s="13">
         <v>124523</v>
       </c>
-      <c r="N8" s="12" t="s">
+      <c r="O8" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P8" s="12" t="s">
+      <c r="Q8" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="Q8" s="4" t="s">
+      <c r="R8" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="R8" s="9" t="s">
+      <c r="S8" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="S8" s="4">
+      <c r="T8" s="4">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:21">
       <c r="A9" s="1">
         <v>62</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
+        <v>7</v>
+      </c>
+      <c r="D9" s="2">
         <v>1311525</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>1311523</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="4">
+      <c r="I9" s="4">
         <v>24651456</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J9" s="3">
+      <c r="K9" s="3">
         <v>43</v>
       </c>
-      <c r="K9" s="3">
+      <c r="L9" s="3">
         <v>84</v>
       </c>
-      <c r="L9" s="5">
+      <c r="M9" s="5">
         <v>42369</v>
       </c>
-      <c r="M9" s="13">
+      <c r="N9" s="13">
         <v>421351</v>
       </c>
-      <c r="N9" s="12" t="s">
+      <c r="O9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P9" s="12" t="s">
+      <c r="Q9" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="Q9" s="4" t="s">
+      <c r="R9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="R9" s="9" t="s">
+      <c r="S9" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="S9" s="4">
+      <c r="T9" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="28">
+    <row r="10" spans="1:21" ht="28">
       <c r="A10" s="1">
         <v>63</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2">
         <v>1311526</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>1311523</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H10" s="4">
+      <c r="I10" s="4">
         <v>24651456</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="3">
+      <c r="K10" s="3">
         <v>59</v>
       </c>
-      <c r="K10" s="3">
+      <c r="L10" s="3">
         <v>72</v>
       </c>
-      <c r="L10" s="5">
+      <c r="M10" s="5">
         <v>42369</v>
       </c>
-      <c r="M10" s="13">
+      <c r="N10" s="13">
         <v>1234</v>
       </c>
-      <c r="N10" s="12" t="s">
+      <c r="O10" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P10" s="12" t="s">
+      <c r="Q10" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="Q10" s="4" t="s">
+      <c r="R10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="R10" s="9" t="s">
+      <c r="S10" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="S10" s="4">
+      <c r="T10" s="4">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:21">
       <c r="A11" s="1">
         <v>64</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2">
         <v>1311527</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>1311523</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="J11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J11" s="3">
+      <c r="K11" s="3">
         <v>34</v>
       </c>
-      <c r="K11" s="3">
+      <c r="L11" s="3">
         <v>45</v>
       </c>
-      <c r="L11" s="5">
+      <c r="M11" s="5">
         <v>42369</v>
       </c>
-      <c r="M11" s="13">
+      <c r="N11" s="13">
         <v>45324</v>
       </c>
-      <c r="N11" s="12" t="s">
+      <c r="O11" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="P11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P11" s="12" t="s">
+      <c r="Q11" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="Q11" s="4" t="s">
+      <c r="R11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="R11" s="9" t="s">
+      <c r="S11" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="S11" s="4">
+      <c r="T11" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:21">
       <c r="A12" s="1">
         <v>65</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2">
         <v>1311528</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>1311523</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="J12" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M12" s="5">
         <v>42369</v>
       </c>
-      <c r="M12" s="13">
+      <c r="N12" s="13">
         <v>482215</v>
       </c>
-      <c r="N12" s="12" t="s">
+      <c r="O12" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P12" s="12" t="s">
+      <c r="Q12" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="Q12" s="4" t="s">
+      <c r="R12" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="R12" s="9" t="s">
+      <c r="S12" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="S12" s="4">
+      <c r="T12" s="4">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:21">
       <c r="A13" s="1">
         <v>66</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
+        <v>10</v>
+      </c>
+      <c r="D13" s="2">
         <v>6798215</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="J13" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="J13" s="3">
+      <c r="K13" s="3">
         <v>88</v>
       </c>
-      <c r="K13" s="3">
+      <c r="L13" s="3">
         <v>942</v>
       </c>
-      <c r="L13" s="5">
+      <c r="M13" s="5">
         <v>42369</v>
       </c>
-      <c r="M13" s="14">
+      <c r="N13" s="14">
         <v>24523</v>
       </c>
-      <c r="N13" s="8" t="s">
+      <c r="O13" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>71</v>
       </c>
-      <c r="P13" s="8" t="s">
+      <c r="Q13" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="Q13" s="4" t="s">
+      <c r="R13" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="R13" s="9" t="s">
+      <c r="S13" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="S13" s="4">
+      <c r="T13" s="4">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="C2:IV1452">
-    <sortCondition ref="C2:C1452"/>
+  <sortState ref="D2:IW1452">
+    <sortCondition ref="D2:D1452"/>
   </sortState>
-  <conditionalFormatting sqref="C2:E2 E3:E4 C9 C11 C5:E6 C7 E7:E13">
+  <conditionalFormatting sqref="D2:F2 F3:F4 D9 D11 D5:F6 D7 F7:F13">
     <cfRule type="duplicateValues" dxfId="2" priority="97"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8 C10 C12">
+  <conditionalFormatting sqref="D8 D10 D12">
     <cfRule type="duplicateValues" dxfId="1" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
+  <conditionalFormatting sqref="D13">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
return naive timestamps for release_date, generation_date, and reccent_sale_date
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="8720" tabRatio="151"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28360" tabRatio="151"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="99">
   <si>
     <t>521 Elm Street</t>
   </si>
@@ -307,6 +307,15 @@
   </si>
   <si>
     <t>jurisdiction property identifier</t>
+  </si>
+  <si>
+    <t>Recent Sale Date</t>
+  </si>
+  <si>
+    <t>Generation Date</t>
+  </si>
+  <si>
+    <t>Release Date</t>
   </si>
 </sst>
 </file>
@@ -393,7 +402,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="80">
+  <cellStyleXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -474,8 +483,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -516,8 +533,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="80">
+  <cellStyles count="88">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -558,6 +577,10 @@
     <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -597,6 +620,10 @@
     <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -930,9 +957,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3:T15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -950,10 +979,14 @@
     <col min="13" max="13" width="11.83203125" style="15" bestFit="1" customWidth="1"/>
     <col min="14" max="16" width="13.5" style="15" customWidth="1"/>
     <col min="17" max="17" width="39" style="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.83203125" style="12"/>
+    <col min="18" max="18" width="11.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11" style="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="8.83203125" style="12"/>
+    <col min="25" max="16384" width="8.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="12">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="12">
       <c r="A1" s="23" t="s">
         <v>95</v>
       </c>
@@ -1006,14 +1039,22 @@
         <v>91</v>
       </c>
       <c r="R1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="U1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="T1" s="4"/>
-    </row>
-    <row r="2" spans="1:20" s="5" customFormat="1">
+    </row>
+    <row r="2" spans="1:22" s="5" customFormat="1">
       <c r="B2" s="5">
         <v>1</v>
       </c>
@@ -1060,15 +1101,23 @@
       <c r="Q2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="R2" s="24">
+        <v>42740.333333333336</v>
+      </c>
+      <c r="S2" s="25">
+        <v>42891.739583333336</v>
+      </c>
+      <c r="T2" s="25">
+        <v>42987.961805555555</v>
+      </c>
+      <c r="U2" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="S2" s="7">
+      <c r="V2" s="7">
         <v>1</v>
       </c>
-      <c r="T2" s="7"/>
-    </row>
-    <row r="3" spans="1:20" s="5" customFormat="1">
+    </row>
+    <row r="3" spans="1:22" s="5" customFormat="1">
       <c r="B3" s="5">
         <v>4</v>
       </c>
@@ -1115,15 +1164,23 @@
       <c r="Q3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="9" t="s">
+      <c r="R3" s="24">
+        <v>42740.333333333336</v>
+      </c>
+      <c r="S3" s="25">
+        <v>42891.739583333336</v>
+      </c>
+      <c r="T3" s="25">
+        <v>42987.961805555555</v>
+      </c>
+      <c r="U3" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="S3" s="7">
+      <c r="V3" s="7">
         <v>4</v>
       </c>
-      <c r="T3" s="7"/>
-    </row>
-    <row r="4" spans="1:20" s="5" customFormat="1">
+    </row>
+    <row r="4" spans="1:22" s="5" customFormat="1">
       <c r="B4" s="5">
         <v>6</v>
       </c>
@@ -1172,15 +1229,23 @@
       <c r="Q4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="9" t="s">
+      <c r="R4" s="24">
+        <v>42740.333333333336</v>
+      </c>
+      <c r="S4" s="25">
+        <v>42891.739583333336</v>
+      </c>
+      <c r="T4" s="25">
+        <v>42987.961805555555</v>
+      </c>
+      <c r="U4" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="S4" s="7">
+      <c r="V4" s="7">
         <v>6</v>
       </c>
-      <c r="T4" s="12"/>
-    </row>
-    <row r="5" spans="1:20" s="5" customFormat="1">
+    </row>
+    <row r="5" spans="1:22" s="5" customFormat="1">
       <c r="B5" s="5">
         <v>7</v>
       </c>
@@ -1229,15 +1294,23 @@
       <c r="Q5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="R5" s="24">
+        <v>42740.333333333336</v>
+      </c>
+      <c r="S5" s="25">
+        <v>42891.739583333336</v>
+      </c>
+      <c r="T5" s="25">
+        <v>42987.961805555555</v>
+      </c>
+      <c r="U5" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="S5" s="7">
+      <c r="V5" s="7">
         <v>7</v>
       </c>
-      <c r="T5" s="12"/>
-    </row>
-    <row r="6" spans="1:20" s="5" customFormat="1">
+    </row>
+    <row r="6" spans="1:22" s="5" customFormat="1">
       <c r="B6" s="5">
         <v>11</v>
       </c>
@@ -1286,15 +1359,23 @@
       <c r="Q6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="R6" s="24">
+        <v>42740.333333333336</v>
+      </c>
+      <c r="S6" s="25">
+        <v>42891.739583333336</v>
+      </c>
+      <c r="T6" s="25">
+        <v>42987.961805555555</v>
+      </c>
+      <c r="U6" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="S6" s="7">
+      <c r="V6" s="7">
         <v>8</v>
       </c>
-      <c r="T6" s="12"/>
-    </row>
-    <row r="7" spans="1:20">
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" s="5"/>
       <c r="B7" s="5">
         <v>8</v>
@@ -1344,14 +1425,23 @@
       <c r="Q7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="R7" s="9" t="s">
+      <c r="R7" s="24">
+        <v>42740.333333333336</v>
+      </c>
+      <c r="S7" s="25">
+        <v>42891.739583333336</v>
+      </c>
+      <c r="T7" s="25">
+        <v>42987.961805555555</v>
+      </c>
+      <c r="U7" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="S7" s="7">
+      <c r="V7" s="7">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:22">
       <c r="A8" s="5"/>
       <c r="B8" s="5">
         <v>9</v>
@@ -1401,14 +1491,23 @@
       <c r="Q8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="R8" s="9" t="s">
+      <c r="R8" s="24">
+        <v>42740.333333333336</v>
+      </c>
+      <c r="S8" s="25">
+        <v>42891.739583333336</v>
+      </c>
+      <c r="T8" s="25">
+        <v>42987.961805555555</v>
+      </c>
+      <c r="U8" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="S8" s="7">
+      <c r="V8" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:22">
       <c r="A9" s="5"/>
       <c r="B9" s="5">
         <v>12</v>
@@ -1458,14 +1557,23 @@
       <c r="Q9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="R9" s="9" t="s">
+      <c r="R9" s="24">
+        <v>42740.333333333336</v>
+      </c>
+      <c r="S9" s="25">
+        <v>42891.739583333336</v>
+      </c>
+      <c r="T9" s="25">
+        <v>42987.961805555555</v>
+      </c>
+      <c r="U9" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="S9" s="7">
+      <c r="V9" s="7">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:22">
       <c r="A10" s="5"/>
       <c r="B10" s="5">
         <v>2</v>
@@ -1513,15 +1621,23 @@
       <c r="Q10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="R10" s="9" t="s">
+      <c r="R10" s="24">
+        <v>42740.333333333336</v>
+      </c>
+      <c r="S10" s="25">
+        <v>42891.739583333336</v>
+      </c>
+      <c r="T10" s="25">
+        <v>42987.961805555555</v>
+      </c>
+      <c r="U10" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="S10" s="7">
+      <c r="V10" s="7">
         <v>2</v>
       </c>
-      <c r="T10" s="7"/>
-    </row>
-    <row r="11" spans="1:20">
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11" s="5"/>
       <c r="B11" s="5">
         <v>3</v>
@@ -1569,15 +1685,23 @@
       <c r="Q11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="R11" s="9" t="s">
+      <c r="R11" s="24">
+        <v>42740.333333333336</v>
+      </c>
+      <c r="S11" s="25">
+        <v>42891.739583333336</v>
+      </c>
+      <c r="T11" s="25">
+        <v>42987.961805555555</v>
+      </c>
+      <c r="U11" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="S11" s="7">
+      <c r="V11" s="7">
         <v>3</v>
       </c>
-      <c r="T11" s="7"/>
-    </row>
-    <row r="12" spans="1:20">
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" s="5"/>
       <c r="B12" s="5">
         <v>5</v>
@@ -1625,15 +1749,23 @@
       <c r="Q12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R12" s="9" t="s">
+      <c r="R12" s="24">
+        <v>42740.333333333336</v>
+      </c>
+      <c r="S12" s="25">
+        <v>42891.739583333336</v>
+      </c>
+      <c r="T12" s="25">
+        <v>42987.961805555555</v>
+      </c>
+      <c r="U12" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="S12" s="7">
+      <c r="V12" s="7">
         <v>5</v>
       </c>
-      <c r="T12" s="7"/>
-    </row>
-    <row r="13" spans="1:20">
+    </row>
+    <row r="13" spans="1:22">
       <c r="B13" s="5">
         <v>10</v>
       </c>
@@ -1679,14 +1811,23 @@
       <c r="Q13" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="R13" s="9" t="s">
+      <c r="R13" s="24">
+        <v>42740.333333333336</v>
+      </c>
+      <c r="S13" s="25">
+        <v>42891.739583333336</v>
+      </c>
+      <c r="T13" s="25">
+        <v>42987.961805555555</v>
+      </c>
+      <c r="U13" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="S13" s="7">
+      <c r="V13" s="7">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:22">
       <c r="A14" s="17"/>
       <c r="B14" s="17">
         <v>13</v>
@@ -1734,15 +1875,23 @@
       <c r="Q14" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="R14" s="22" t="s">
+      <c r="R14" s="24">
+        <v>42740.333333333336</v>
+      </c>
+      <c r="S14" s="25">
+        <v>42891.739583333336</v>
+      </c>
+      <c r="T14" s="25">
+        <v>42987.961805555555</v>
+      </c>
+      <c r="U14" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="S14" s="17">
+      <c r="V14" s="17">
         <v>10</v>
       </c>
-      <c r="T14" s="17"/>
-    </row>
-    <row r="15" spans="1:20">
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" s="17"/>
       <c r="B15" s="17">
         <v>13</v>
@@ -1790,13 +1939,21 @@
       <c r="Q15" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="R15" s="22" t="s">
+      <c r="R15" s="24">
+        <v>42740.333333333336</v>
+      </c>
+      <c r="S15" s="25">
+        <v>42891.739583333336</v>
+      </c>
+      <c r="T15" s="25">
+        <v>42987.961805555555</v>
+      </c>
+      <c r="U15" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="S15" s="17">
+      <c r="V15" s="17">
         <v>11</v>
       </c>
-      <c r="T15" s="17"/>
     </row>
     <row r="17" spans="8:8">
       <c r="H17" s="7"/>

</xml_diff>

<commit_message>
is_espm is not a database fieldgs
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28360" tabRatio="151"/>
+    <workbookView xWindow="0" yWindow="14140" windowWidth="51200" windowHeight="14140" tabRatio="151"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="100">
   <si>
     <t>521 Elm Street</t>
   </si>
@@ -316,6 +316,9 @@
   </si>
   <si>
     <t>Release Date</t>
+  </si>
+  <si>
+    <t>1/5/1888 08:00</t>
   </si>
 </sst>
 </file>
@@ -402,7 +405,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="88">
+  <cellStyleXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -491,8 +494,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -535,8 +540,11 @@
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="88">
+  <cellStyles count="90">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -581,6 +589,7 @@
     <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -624,6 +633,7 @@
     <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -959,8 +969,8 @@
   </sheetPr>
   <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3:T15"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -979,7 +989,7 @@
     <col min="13" max="13" width="11.83203125" style="15" bestFit="1" customWidth="1"/>
     <col min="14" max="16" width="13.5" style="15" customWidth="1"/>
     <col min="17" max="17" width="39" style="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.1640625" style="12" customWidth="1"/>
     <col min="19" max="19" width="11.6640625" style="12" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" style="12" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="8.83203125" style="12"/>
@@ -1101,8 +1111,8 @@
       <c r="Q2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="24">
-        <v>42740.333333333336</v>
+      <c r="R2" s="26" t="s">
+        <v>99</v>
       </c>
       <c r="S2" s="25">
         <v>42891.739583333336</v>

</xml_diff>

<commit_message>
fix strftime issue with dates before 1900
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties.xlsx
@@ -309,16 +309,16 @@
     <t>jurisdiction property identifier</t>
   </si>
   <si>
-    <t>Recent Sale Date</t>
-  </si>
-  <si>
-    <t>Generation Date</t>
-  </si>
-  <si>
-    <t>Release Date</t>
-  </si>
-  <si>
     <t>1/5/1888 08:00</t>
+  </si>
+  <si>
+    <t>recent sale date</t>
+  </si>
+  <si>
+    <t>generation date</t>
+  </si>
+  <si>
+    <t>release date</t>
   </si>
 </sst>
 </file>
@@ -970,7 +970,7 @@
   <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1049,13 +1049,13 @@
         <v>91</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="U1" s="4" t="s">
         <v>92</v>
@@ -1112,7 +1112,7 @@
         <v>3</v>
       </c>
       <c r="R2" s="26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="S2" s="25">
         <v>42891.739583333336</v>
@@ -1239,9 +1239,7 @@
       <c r="Q4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="24">
-        <v>42740.333333333336</v>
-      </c>
+      <c r="R4" s="24"/>
       <c r="S4" s="25">
         <v>42891.739583333336</v>
       </c>

</xml_diff>

<commit_message>
taxlot history cleanup and tests
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="28260" tabRatio="151"/>
+    <workbookView xWindow="25600" yWindow="440" windowWidth="25600" windowHeight="28260" tabRatio="151"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -458,9 +458,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="90">
+  <cellStyleXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -597,7 +601,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="90">
+  <cellStyles count="94">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -643,6 +647,8 @@
     <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -687,6 +693,8 @@
     <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -1022,8 +1030,8 @@
   </sheetPr>
   <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added postal code column for testing
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10610"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlong/working/seed/seed/data_importer/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/llin/Documents/repo/seed/seed/data_importer/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEE6226-E6BA-7643-A5FF-5E051FA10A98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A77FA4-A4D8-A04C-ABEB-F52B069EDE3E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="14620" windowWidth="51200" windowHeight="14180" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37680" yWindow="2940" windowWidth="51200" windowHeight="14180" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="119">
   <si>
     <t>521 Elm Street</t>
   </si>
@@ -379,15 +379,22 @@
   </si>
   <si>
     <t>86HJX838+8M7-1-3-1-2</t>
+  </si>
+  <si>
+    <t>postal code</t>
+  </si>
+  <si>
+    <t>123-45</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="00000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -561,7 +568,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -607,6 +614,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="94">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1038,10 +1049,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Y23"/>
+  <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="Z16" sqref="Z16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1068,10 +1079,11 @@
     <col min="22" max="22" width="11" style="12" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.83203125" style="12" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="8.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.83203125" style="12"/>
+    <col min="26" max="26" width="11.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="8.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>95</v>
       </c>
@@ -1147,8 +1159,11 @@
       <c r="Y1" s="4" t="s">
         <v>93</v>
       </c>
+      <c r="Z1" s="27" t="s">
+        <v>117</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5">
         <v>1</v>
       </c>
@@ -1219,8 +1234,11 @@
       <c r="Y2" s="7">
         <v>1</v>
       </c>
+      <c r="Z2" s="5" t="s">
+        <v>118</v>
+      </c>
     </row>
-    <row r="3" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5">
         <v>4</v>
       </c>
@@ -1291,8 +1309,11 @@
       <c r="Y3" s="7">
         <v>4</v>
       </c>
+      <c r="Z3" s="28">
+        <v>801</v>
+      </c>
     </row>
-    <row r="4" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5">
         <v>6</v>
       </c>
@@ -1363,8 +1384,11 @@
       <c r="Y4" s="7">
         <v>6</v>
       </c>
+      <c r="Z4" s="28">
+        <v>802</v>
+      </c>
     </row>
-    <row r="5" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5">
         <v>7</v>
       </c>
@@ -1437,8 +1461,11 @@
       <c r="Y5" s="7">
         <v>7</v>
       </c>
+      <c r="Z5" s="28">
+        <v>803</v>
+      </c>
     </row>
-    <row r="6" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5">
         <v>11</v>
       </c>
@@ -1511,8 +1538,11 @@
       <c r="Y6" s="7">
         <v>8</v>
       </c>
+      <c r="Z6" s="28">
+        <v>804</v>
+      </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="5">
         <v>8</v>
@@ -1586,8 +1616,11 @@
       <c r="Y7" s="7">
         <v>9</v>
       </c>
+      <c r="Z7" s="28">
+        <v>805</v>
+      </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="5">
         <v>9</v>
@@ -1661,8 +1694,11 @@
       <c r="Y8" s="7">
         <v>10</v>
       </c>
+      <c r="Z8" s="28">
+        <v>806</v>
+      </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="5">
         <v>12</v>
@@ -1736,8 +1772,11 @@
       <c r="Y9" s="7">
         <v>11</v>
       </c>
+      <c r="Z9" s="28">
+        <v>807</v>
+      </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="5">
         <v>2</v>
@@ -1809,8 +1848,11 @@
       <c r="Y10" s="7">
         <v>2</v>
       </c>
+      <c r="Z10" s="28">
+        <v>808</v>
+      </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="5">
         <v>3</v>
@@ -1882,8 +1924,11 @@
       <c r="Y11" s="7">
         <v>3</v>
       </c>
+      <c r="Z11" s="28">
+        <v>809</v>
+      </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="5">
         <v>5</v>
@@ -1955,8 +2000,11 @@
       <c r="Y12" s="7">
         <v>5</v>
       </c>
+      <c r="Z12" s="28">
+        <v>80901</v>
+      </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B13" s="5">
         <v>10</v>
       </c>
@@ -2026,8 +2074,11 @@
       <c r="Y13" s="7">
         <v>12</v>
       </c>
+      <c r="Z13" s="28">
+        <v>80902</v>
+      </c>
     </row>
-    <row r="14" spans="1:25" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="17">
         <v>13</v>
@@ -2099,8 +2150,11 @@
       <c r="Y14" s="17">
         <v>10</v>
       </c>
+      <c r="Z14" s="28">
+        <v>80903</v>
+      </c>
     </row>
-    <row r="15" spans="1:25" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="17">
         <v>13</v>
@@ -2172,8 +2226,11 @@
       <c r="Y15" s="17">
         <v>11</v>
       </c>
+      <c r="Z15" s="28">
+        <v>80904</v>
+      </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="E16"/>
     </row>
     <row r="17" spans="5:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
more data property xlsx file modification for testing
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/llin/Documents/repo/seed/seed/data_importer/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A691DD-8829-9448-9E63-7A43FC092A65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9660D094-D31C-8E4B-8655-80E23B8CC02C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42140" yWindow="680" windowWidth="28800" windowHeight="16440" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16360" yWindow="800" windowWidth="28800" windowHeight="16440" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -1040,7 +1040,7 @@
   </sheetPr>
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
@@ -1470,7 +1470,7 @@
         <v>43</v>
       </c>
       <c r="L6" s="7">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M6" s="8">
         <v>42369</v>
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="L10" s="7">
-        <v>-10</v>
+        <v>70</v>
       </c>
       <c r="M10" s="8">
         <v>42369</v>
@@ -1985,7 +1985,7 @@
         <v>88</v>
       </c>
       <c r="L13" s="7">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="M13" s="8">
         <v>42369</v>
@@ -2058,7 +2058,7 @@
         <v>34</v>
       </c>
       <c r="L14" s="7">
-        <v>65</v>
+        <v>-10</v>
       </c>
       <c r="M14" s="19">
         <v>42369</v>
@@ -2131,7 +2131,7 @@
         <v>32</v>
       </c>
       <c r="L15" s="7">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="M15" s="19">
         <v>42369</v>

</xml_diff>

<commit_message>
Modified example-data_properties.xlsx for testing purposes
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/llin/Documents/repo/seed/seed/data_importer/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9660D094-D31C-8E4B-8655-80E23B8CC02C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F746E511-3283-A645-B127-F36CD2F76423}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16360" yWindow="800" windowWidth="28800" windowHeight="16440" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39540" yWindow="960" windowWidth="28800" windowHeight="16440" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="117">
   <si>
     <t>521 Elm Street</t>
   </si>
@@ -1040,8 +1040,8 @@
   </sheetPr>
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1178,7 +1178,7 @@
         <v>75</v>
       </c>
       <c r="L2" s="6">
-        <v>50</v>
+        <v>125</v>
       </c>
       <c r="M2" s="8">
         <v>42369</v>
@@ -1914,7 +1914,7 @@
         <v>55</v>
       </c>
       <c r="L12" s="7">
-        <v>101</v>
+        <v>1358</v>
       </c>
       <c r="M12" s="8">
         <v>42369</v>
@@ -2127,8 +2127,8 @@
       <c r="J15" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="K15" s="17" t="s">
-        <v>32</v>
+      <c r="K15" s="17">
+        <v>60</v>
       </c>
       <c r="L15" s="7">
         <v>65</v>

</xml_diff>

<commit_message>
chore: merge develop into bricr-dev
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlong/working/seed/seed/data_importer/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/llin/Documents/repo/seed/seed/data_importer/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEE6226-E6BA-7643-A5FF-5E051FA10A98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F746E511-3283-A645-B127-F36CD2F76423}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="14620" windowWidth="51200" windowHeight="14180" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39540" yWindow="960" windowWidth="28800" windowHeight="16440" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="117">
   <si>
     <t>521 Elm Street</t>
   </si>
@@ -1040,8 +1040,8 @@
   </sheetPr>
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1177,7 +1177,7 @@
       <c r="K2" s="7">
         <v>75</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="6">
         <v>125</v>
       </c>
       <c r="M2" s="8">
@@ -1323,8 +1323,8 @@
       <c r="K4" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="5" t="s">
-        <v>32</v>
+      <c r="L4" s="7">
+        <v>300</v>
       </c>
       <c r="M4" s="8">
         <v>42369</v>
@@ -1396,7 +1396,7 @@
         <v>77</v>
       </c>
       <c r="L5" s="7">
-        <v>219</v>
+        <v>45</v>
       </c>
       <c r="M5" s="8">
         <v>42369</v>
@@ -1470,7 +1470,7 @@
         <v>43</v>
       </c>
       <c r="L6" s="7">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="M6" s="8">
         <v>42369</v>
@@ -1545,7 +1545,7 @@
         <v>59</v>
       </c>
       <c r="L7" s="7">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="M7" s="8">
         <v>42369</v>
@@ -1620,7 +1620,7 @@
         <v>34</v>
       </c>
       <c r="L8" s="7">
-        <v>45</v>
+        <v>2906</v>
       </c>
       <c r="M8" s="8">
         <v>42369</v>
@@ -1694,8 +1694,8 @@
       <c r="K9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>32</v>
+      <c r="L9" s="7">
+        <v>0</v>
       </c>
       <c r="M9" s="8">
         <v>42369</v>
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="L10" s="7">
-        <v>652.29999999999995</v>
+        <v>70</v>
       </c>
       <c r="M10" s="8">
         <v>42369</v>
@@ -1840,8 +1840,8 @@
       <c r="K11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>32</v>
+      <c r="L11" s="7">
+        <v>29</v>
       </c>
       <c r="M11" s="8">
         <v>42369</v>
@@ -1985,7 +1985,7 @@
         <v>88</v>
       </c>
       <c r="L13" s="7">
-        <v>942</v>
+        <v>50</v>
       </c>
       <c r="M13" s="8">
         <v>42369</v>
@@ -2057,8 +2057,8 @@
       <c r="K14" s="18">
         <v>34</v>
       </c>
-      <c r="L14" s="18">
-        <v>45</v>
+      <c r="L14" s="7">
+        <v>-10</v>
       </c>
       <c r="M14" s="19">
         <v>42369</v>
@@ -2127,11 +2127,11 @@
       <c r="J15" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="K15" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="L15" s="17" t="s">
-        <v>32</v>
+      <c r="K15" s="17">
+        <v>60</v>
+      </c>
+      <c r="L15" s="7">
+        <v>65</v>
       </c>
       <c r="M15" s="19">
         <v>42369</v>
@@ -2205,7 +2205,7 @@
       <c r="I23" s="5"/>
     </row>
   </sheetData>
-  <sortState ref="A2:V13">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V13">
     <sortCondition ref="B2:B13"/>
   </sortState>
   <conditionalFormatting sqref="C2:D2 C9 C11 C5:D6 C7 F2:F13">

</xml_diff>

<commit_message>
add property timezone as a canonical database field
</commit_message>
<xml_diff>
--- a/seed/data_importer/tests/data/example-data-properties.xlsx
+++ b/seed/data_importer/tests/data/example-data-properties.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10520"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/llin/Documents/repo/seed/seed/data_importer/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nlong/working/seed/seed/seed/data_importer/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F746E511-3283-A645-B127-F36CD2F76423}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DF6942-A42D-AF43-82C6-ED742172C904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39540" yWindow="960" windowWidth="28800" windowHeight="16440" tabRatio="151" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="119">
   <si>
     <t>521 Elm Street</t>
   </si>
@@ -379,6 +379,12 @@
   </si>
   <si>
     <t>86HJX838+8M7-1-3-1-2</t>
+  </si>
+  <si>
+    <t>property timezone</t>
+  </si>
+  <si>
+    <t>US/Mountain</t>
   </si>
 </sst>
 </file>
@@ -1038,10 +1044,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Y23"/>
+  <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2:U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1064,14 +1070,15 @@
     <col min="17" max="17" width="12.6640625" style="15" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="39.1640625" style="12" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="8.83203125" style="12"/>
-    <col min="21" max="21" width="12.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11" style="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="8.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.83203125" style="12"/>
+    <col min="21" max="21" width="13" style="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" style="12" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="8.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="8.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>95</v>
       </c>
@@ -1132,23 +1139,26 @@
       <c r="T1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="5">
         <v>1</v>
       </c>
@@ -1204,23 +1214,26 @@
       <c r="T2" s="5">
         <v>-105.22110000000001</v>
       </c>
-      <c r="U2" s="26" t="s">
+      <c r="U2" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="V2" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="V2" s="25">
+      <c r="W2" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W2" s="25">
+      <c r="X2" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="Y2" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="Y2" s="7">
+      <c r="Z2" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5">
         <v>4</v>
       </c>
@@ -1276,23 +1289,26 @@
       <c r="T3" s="5">
         <v>-105.225381</v>
       </c>
-      <c r="U3" s="24">
+      <c r="U3" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="V3" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V3" s="25">
+      <c r="W3" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W3" s="25">
+      <c r="X3" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X3" s="9" t="s">
+      <c r="Y3" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="Y3" s="7">
+      <c r="Z3" s="7">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5">
         <v>6</v>
       </c>
@@ -1350,21 +1366,24 @@
       <c r="T4" s="5">
         <v>-105.17121</v>
       </c>
-      <c r="U4" s="24"/>
-      <c r="V4" s="25">
+      <c r="U4" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="V4" s="24"/>
+      <c r="W4" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W4" s="25">
+      <c r="X4" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X4" s="9" t="s">
+      <c r="Y4" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="Y4" s="7">
+      <c r="Z4" s="7">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5">
         <v>7</v>
       </c>
@@ -1422,23 +1441,26 @@
       <c r="T5" s="5">
         <v>-105.159808</v>
       </c>
-      <c r="U5" s="24">
+      <c r="U5" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="V5" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V5" s="25">
+      <c r="W5" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W5" s="25">
+      <c r="X5" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X5" s="9" t="s">
+      <c r="Y5" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="Y5" s="7">
+      <c r="Z5" s="7">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5">
         <v>11</v>
       </c>
@@ -1496,23 +1518,26 @@
       <c r="T6" s="5">
         <v>-105.162576</v>
       </c>
-      <c r="U6" s="24">
+      <c r="U6" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="V6" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V6" s="25">
+      <c r="W6" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W6" s="25">
+      <c r="X6" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X6" s="9" t="s">
+      <c r="Y6" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="Y6" s="7">
+      <c r="Z6" s="7">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="5">
         <v>8</v>
@@ -1571,23 +1596,26 @@
       <c r="T7" s="12">
         <v>-104.984951</v>
       </c>
-      <c r="U7" s="24">
+      <c r="U7" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="V7" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V7" s="25">
+      <c r="W7" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W7" s="25">
+      <c r="X7" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X7" s="9" t="s">
+      <c r="Y7" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="Y7" s="7">
+      <c r="Z7" s="7">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="5">
         <v>9</v>
@@ -1646,23 +1674,26 @@
       <c r="T8" s="12">
         <v>-104.96074299999999</v>
       </c>
-      <c r="U8" s="24">
+      <c r="U8" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="V8" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V8" s="25">
+      <c r="W8" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W8" s="25">
+      <c r="X8" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X8" s="9" t="s">
+      <c r="Y8" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="Y8" s="7">
+      <c r="Z8" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="5">
         <v>12</v>
@@ -1721,23 +1752,26 @@
       <c r="T9" s="12">
         <v>-104.975129</v>
       </c>
-      <c r="U9" s="24">
+      <c r="U9" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="V9" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V9" s="25">
+      <c r="W9" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W9" s="25">
+      <c r="X9" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X9" s="9" t="s">
+      <c r="Y9" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="Y9" s="7">
+      <c r="Z9" s="7">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="5">
         <v>2</v>
@@ -1794,23 +1828,26 @@
       <c r="T10" s="12">
         <v>-104.996673</v>
       </c>
-      <c r="U10" s="24">
+      <c r="U10" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="V10" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V10" s="25">
+      <c r="W10" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W10" s="25">
+      <c r="X10" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X10" s="9" t="s">
+      <c r="Y10" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="Y10" s="7">
+      <c r="Z10" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="5">
         <v>3</v>
@@ -1867,23 +1904,26 @@
       <c r="T11" s="12">
         <v>-105.270546</v>
       </c>
-      <c r="U11" s="24">
+      <c r="U11" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="V11" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V11" s="25">
+      <c r="W11" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W11" s="25">
+      <c r="X11" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X11" s="9" t="s">
+      <c r="Y11" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="Y11" s="7">
+      <c r="Z11" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="5">
         <v>5</v>
@@ -1940,23 +1980,26 @@
       <c r="T12" s="12">
         <v>-105.26486800000001</v>
       </c>
-      <c r="U12" s="24">
+      <c r="U12" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="V12" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V12" s="25">
+      <c r="W12" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W12" s="25">
+      <c r="X12" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X12" s="9" t="s">
+      <c r="Y12" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="Y12" s="7">
+      <c r="Z12" s="7">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B13" s="5">
         <v>10</v>
       </c>
@@ -2011,23 +2054,26 @@
       <c r="T13" s="12">
         <v>-105.26242000000001</v>
       </c>
-      <c r="U13" s="24">
+      <c r="U13" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="V13" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V13" s="25">
+      <c r="W13" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W13" s="25">
+      <c r="X13" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X13" s="9" t="s">
+      <c r="Y13" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="Y13" s="7">
+      <c r="Z13" s="7">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="17">
         <v>13</v>
@@ -2084,23 +2130,26 @@
       <c r="T14" s="12">
         <v>-105.02010900000001</v>
       </c>
-      <c r="U14" s="24">
+      <c r="U14" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="V14" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V14" s="25">
+      <c r="W14" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W14" s="25">
+      <c r="X14" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X14" s="22" t="s">
+      <c r="Y14" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="Y14" s="17">
+      <c r="Z14" s="17">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="17">
         <v>13</v>
@@ -2157,23 +2206,26 @@
       <c r="T15" s="12">
         <v>-105.007644</v>
       </c>
-      <c r="U15" s="24">
+      <c r="U15" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="V15" s="24">
         <v>42740.333333333336</v>
       </c>
-      <c r="V15" s="25">
+      <c r="W15" s="25">
         <v>42891.739583333336</v>
       </c>
-      <c r="W15" s="25">
+      <c r="X15" s="25">
         <v>42987.961805555555</v>
       </c>
-      <c r="X15" s="22" t="s">
+      <c r="Y15" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="Y15" s="17">
+      <c r="Z15" s="17">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="E16"/>
     </row>
     <row r="17" spans="5:9" x14ac:dyDescent="0.2">
@@ -2205,7 +2257,7 @@
       <c r="I23" s="5"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V13">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:W13">
     <sortCondition ref="B2:B13"/>
   </sortState>
   <conditionalFormatting sqref="C2:D2 C9 C11 C5:D6 C7 F2:F13">

</xml_diff>